<commit_message>
Added TC003 and Test data in data.xlsx
</commit_message>
<xml_diff>
--- a/Guru99/datadriven/data.xlsx
+++ b/Guru99/datadriven/data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="22980" windowHeight="9288" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="New customer" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Negative Testing" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>saan</t>
   </si>
@@ -25,16 +25,33 @@
   </si>
   <si>
     <t>santoshshrinivasshriramoj</t>
+  </si>
+  <si>
+    <t>!@#$%</t>
+  </si>
+  <si>
+    <t>123sasf</t>
+  </si>
+  <si>
+    <t>!@#!123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,13 +74,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,7 +386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -393,12 +414,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1234454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>